<commit_message>
added data + updated spreadsheet
</commit_message>
<xml_diff>
--- a/training_data/data_npd.xlsx
+++ b/training_data/data_npd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabe\Documents\GitHub\Sheet-Music-Project\training_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4810797-2EB6-4CA1-92A9-890DDB799D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F1694B-C55F-41FB-80F6-F88C49A86DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>a3_1</t>
   </si>
@@ -106,6 +106,30 @@
   </si>
   <si>
     <t>c4_3</t>
+  </si>
+  <si>
+    <t>c3_4</t>
+  </si>
+  <si>
+    <t>d3_4</t>
+  </si>
+  <si>
+    <t>e3_4</t>
+  </si>
+  <si>
+    <t>f3_4</t>
+  </si>
+  <si>
+    <t>g3_4</t>
+  </si>
+  <si>
+    <t>a3_4</t>
+  </si>
+  <si>
+    <t>b3_4</t>
+  </si>
+  <si>
+    <t>c4_4</t>
   </si>
 </sst>
 </file>
@@ -423,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,6 +730,94 @@
         <v>2</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>130</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>146</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>164</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>174</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>196</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>208</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>246</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>261</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dur and pitch changes
more duration and pitch changes for rests and quarter notes
</commit_message>
<xml_diff>
--- a/training_data/data_npd.xlsx
+++ b/training_data/data_npd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillav/ECE 1390/Sheet-Music-Project/training_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9F8E69-5572-494D-990A-F5E78B970585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771AD43A-9363-B549-B763-7CEF0A7C920A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="1220" windowWidth="26280" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>a3_1</t>
   </si>
@@ -226,6 +226,30 @@
   </si>
   <si>
     <t>c4_8</t>
+  </si>
+  <si>
+    <t>rest_1</t>
+  </si>
+  <si>
+    <t>rest_2</t>
+  </si>
+  <si>
+    <t>rest_3</t>
+  </si>
+  <si>
+    <t>rest_4</t>
+  </si>
+  <si>
+    <t>rest_5</t>
+  </si>
+  <si>
+    <t>rest_6</t>
+  </si>
+  <si>
+    <t>rest_7</t>
+  </si>
+  <si>
+    <t>rest_8</t>
   </si>
 </sst>
 </file>
@@ -543,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G66" sqref="G14:G66"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -570,7 +594,7 @@
         <v>130</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -581,7 +605,7 @@
         <v>146</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -592,7 +616,7 @@
         <v>164</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -603,7 +627,7 @@
         <v>174</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -614,7 +638,7 @@
         <v>196</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -625,7 +649,7 @@
         <v>220</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -636,7 +660,7 @@
         <v>246</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -647,7 +671,7 @@
         <v>261</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -658,7 +682,7 @@
         <v>130</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -669,7 +693,7 @@
         <v>146</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -680,7 +704,7 @@
         <v>164</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -691,7 +715,7 @@
         <v>174</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -702,7 +726,7 @@
         <v>196</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -713,7 +737,7 @@
         <v>220</v>
       </c>
       <c r="C15">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -724,7 +748,7 @@
         <v>246</v>
       </c>
       <c r="C16">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -735,7 +759,7 @@
         <v>261</v>
       </c>
       <c r="C17">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -746,7 +770,7 @@
         <v>130</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -757,7 +781,7 @@
         <v>146</v>
       </c>
       <c r="C19">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -768,7 +792,7 @@
         <v>164</v>
       </c>
       <c r="C20">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -779,7 +803,7 @@
         <v>174</v>
       </c>
       <c r="C21">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -790,7 +814,7 @@
         <v>196</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -801,7 +825,7 @@
         <v>220</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -812,7 +836,7 @@
         <v>246</v>
       </c>
       <c r="C24">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -823,7 +847,7 @@
         <v>261</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -834,7 +858,7 @@
         <v>130</v>
       </c>
       <c r="C26">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -845,7 +869,7 @@
         <v>146</v>
       </c>
       <c r="C27">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -856,7 +880,7 @@
         <v>164</v>
       </c>
       <c r="C28">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -867,7 +891,7 @@
         <v>174</v>
       </c>
       <c r="C29">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -878,7 +902,7 @@
         <v>196</v>
       </c>
       <c r="C30">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -889,7 +913,7 @@
         <v>220</v>
       </c>
       <c r="C31">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -900,7 +924,7 @@
         <v>246</v>
       </c>
       <c r="C32">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -911,7 +935,7 @@
         <v>261</v>
       </c>
       <c r="C33">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -922,7 +946,7 @@
         <v>130</v>
       </c>
       <c r="C34">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -933,7 +957,7 @@
         <v>146</v>
       </c>
       <c r="C35">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -944,7 +968,7 @@
         <v>164</v>
       </c>
       <c r="C36">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -955,7 +979,7 @@
         <v>174</v>
       </c>
       <c r="C37">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -966,7 +990,7 @@
         <v>196</v>
       </c>
       <c r="C38">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -977,7 +1001,7 @@
         <v>220</v>
       </c>
       <c r="C39">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -988,7 +1012,7 @@
         <v>246</v>
       </c>
       <c r="C40">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -999,7 +1023,7 @@
         <v>261</v>
       </c>
       <c r="C41">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1010,7 +1034,7 @@
         <v>130</v>
       </c>
       <c r="C42">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1021,7 +1045,7 @@
         <v>146</v>
       </c>
       <c r="C43">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1032,7 +1056,7 @@
         <v>164</v>
       </c>
       <c r="C44">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1043,7 +1067,7 @@
         <v>174</v>
       </c>
       <c r="C45">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1054,7 +1078,7 @@
         <v>196</v>
       </c>
       <c r="C46">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1065,7 +1089,7 @@
         <v>220</v>
       </c>
       <c r="C47">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1076,7 +1100,7 @@
         <v>246</v>
       </c>
       <c r="C48">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1087,7 +1111,7 @@
         <v>261</v>
       </c>
       <c r="C49">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1098,7 +1122,7 @@
         <v>130</v>
       </c>
       <c r="C50">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1109,7 +1133,7 @@
         <v>146</v>
       </c>
       <c r="C51">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1120,7 +1144,7 @@
         <v>164</v>
       </c>
       <c r="C52">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1131,7 +1155,7 @@
         <v>174</v>
       </c>
       <c r="C53">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1142,7 +1166,7 @@
         <v>196</v>
       </c>
       <c r="C54">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1153,7 +1177,7 @@
         <v>220</v>
       </c>
       <c r="C55">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1164,7 +1188,7 @@
         <v>246</v>
       </c>
       <c r="C56">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1175,7 +1199,7 @@
         <v>261</v>
       </c>
       <c r="C57">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1186,7 +1210,7 @@
         <v>130</v>
       </c>
       <c r="C58">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1197,7 +1221,7 @@
         <v>146</v>
       </c>
       <c r="C59">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1208,7 +1232,7 @@
         <v>164</v>
       </c>
       <c r="C60">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1219,7 +1243,7 @@
         <v>174</v>
       </c>
       <c r="C61">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1230,7 +1254,7 @@
         <v>196</v>
       </c>
       <c r="C62">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1241,7 +1265,7 @@
         <v>220</v>
       </c>
       <c r="C63">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1252,7 +1276,7 @@
         <v>246</v>
       </c>
       <c r="C64">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1263,7 +1287,95 @@
         <v>261</v>
       </c>
       <c r="C65">
-        <v>0.5</v>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="C66">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="C67">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="C68">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="C69">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="C70">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="C71">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="C72">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="C73">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>